<commit_message>
Added text about cloud security
</commit_message>
<xml_diff>
--- a/documents/cloud_security.xlsx
+++ b/documents/cloud_security.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OWNER\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OWNER\dippa\dippa-teemup\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71992919-3FE1-4EC2-9E14-4FCF1FFE91DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7880AEE-399D-4185-87C1-E081FAEA24C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B7F970F4-B6D3-4245-AC02-779C897EE963}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B7F970F4-B6D3-4245-AC02-779C897EE963}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Pilvitietomurto</t>
   </si>
@@ -94,6 +96,45 @@
   </si>
   <si>
     <t>Varmuuskopioiden turvaton säilyttäminen</t>
+  </si>
+  <si>
+    <t>Riittävän valvonnan puute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ei riittävää ympäristön seurantaa </t>
+  </si>
+  <si>
+    <t>Arkkitehtuurin haavoittuvuuksia ei käsitellä</t>
+  </si>
+  <si>
+    <t>Haitallinen sisäpiirin käyttäytyminen</t>
+  </si>
+  <si>
+    <t>Huolimaton sisäpiirin käyttäytyminen</t>
+  </si>
+  <si>
+    <t>Rajapintojen liiallinen määrä</t>
+  </si>
+  <si>
+    <t>Turvallisuusinvestointien puute</t>
+  </si>
+  <si>
+    <t>Nopea ympäristön muuttuminen</t>
+  </si>
+  <si>
+    <t>Tietämyksen puute</t>
+  </si>
+  <si>
+    <t>Virheet</t>
+  </si>
+  <si>
+    <t>Inhimillinen tekijä</t>
+  </si>
+  <si>
+    <t>Lunnasohjelmat tai kiristys</t>
+  </si>
+  <si>
+    <t>Kolmannen osapuolen palvelut</t>
   </si>
 </sst>
 </file>
@@ -183,7 +224,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1500" baseline="0"/>
-              <a:t>Koetut vakavat pilviturvallisuushäiriöt</a:t>
+              <a:t>Koetut vakavat pilviturvallisuusongelmat</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -566,7 +607,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Tietoturvahäiriön aiheuttaja</a:t>
+              <a:t>Tietoturvaongelman aiheuttaja</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -970,6 +1011,778 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tietoturvaongelmien aiheutumisen syyt</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$1:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Riittävän valvonnan puute</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ei riittävää ympäristön seurantaa </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Arkkitehtuurin haavoittuvuuksia ei käsitellä</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Haitallinen sisäpiirin käyttäytyminen</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Huolimaton sisäpiirin käyttäytyminen</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Rajapintojen liiallinen määrä</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Turvallisuusinvestointien puute</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Nopea ympäristön muuttuminen</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Tietämyksen puute</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$1:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B6B-4982-993E-C1874768D18D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1755276383"/>
+        <c:axId val="1755280703"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1755276383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1755280703"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1755280703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Prosenttiosuus(%) kuinka moni</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> vastaajista on valinnut  vaihtoehdon</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.13439219573077837"/>
+              <c:y val="0.93104575163398695"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1755276383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100" baseline="0"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Avaintekijä</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> tietomurroissa</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$1:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Kolmannen osapuolen palvelut</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Virheet</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lunnasohjelmat tai kiristys</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Inhimillinen tekijä</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$1:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EDD0-4E37-9AA9-D156C6C493AB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="69364911"/>
+        <c:axId val="69370671"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="69364911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69370671"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69370671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>Prosenttiosuus  tietomurroista (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69364911"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1050,6 +1863,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -1556,6 +2449,1016 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2122,6 +4025,88 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1990224C-457D-220E-B4AC-08DA46FC6F41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E8CA35C-55FE-C886-D38D-8E80402BD2E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>176212</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>481012</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5397330-92C2-7F17-9D03-CEF43D0FC725}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2545,7 +4530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2884B403-E7E4-4DD5-BBBD-4D6D77DD3A76}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -2646,4 +4631,149 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D75F87C-72F2-4139-9249-2B5B4734D9B7}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DF97E8-BE24-43D1-85A7-94BE3F5FBFC9}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B4">
+    <sortCondition descending="1" ref="A2:A4"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added text to abstract
</commit_message>
<xml_diff>
--- a/documents/cloud_security.xlsx
+++ b/documents/cloud_security.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OWNER\dippa\dippa-teemup\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7880AEE-399D-4185-87C1-E081FAEA24C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48638B4-01FD-4860-B8CB-152914343D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B7F970F4-B6D3-4245-AC02-779C897EE963}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B7F970F4-B6D3-4245-AC02-779C897EE963}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Pilvitietomurto</t>
   </si>
@@ -135,6 +136,15 @@
   </si>
   <si>
     <t>Kolmannen osapuolen palvelut</t>
+  </si>
+  <si>
+    <t>Käyttäjätunnisteet</t>
+  </si>
+  <si>
+    <t>Tietojenkalastelu</t>
+  </si>
+  <si>
+    <t>Haavoittuvuudet</t>
   </si>
 </sst>
 </file>
@@ -1783,6 +1793,362 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tietomurroissa käytetyt menetelmät</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet5!$A$1:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Tietojenkalastelu</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Haavoittuvuudet</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Käyttäjätunnisteet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$B$1:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-05EF-4948-8078-DF0EDD81C241}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="727599471"/>
+        <c:axId val="727596111"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="727599471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="727596111"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="727596111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>Prosenttiosuus tietomurroista (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="727599471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1943,6 +2309,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -3459,6 +3865,511 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4107,6 +5018,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5397330-92C2-7F17-9D03-CEF43D0FC725}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA29B6E9-D799-5315-6300-74307299B77D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4530,7 +5482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2884B403-E7E4-4DD5-BBBD-4D6D77DD3A76}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -4728,7 +5680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DF97E8-BE24-43D1-85A7-94BE3F5FBFC9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -4776,4 +5728,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A29C67-4E69-41F5-843A-374D57C6831D}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B2">
+    <sortCondition descending="1" ref="A1:A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>